<commit_message>
Datos CSV y definiciones actualizados
</commit_message>
<xml_diff>
--- a/content/excel/Fichas década4 (1920).xlsx
+++ b/content/excel/Fichas década4 (1920).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19320" windowHeight="15480" tabRatio="500" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19320" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ÁREA DE IDENTIFICACIÓN" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="ÁREA DE NOTAS" sheetId="6" r:id="rId6"/>
     <sheet name="ÁREA DE DESCRIPCIÓN" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="223">
   <si>
     <r>
       <rPr>
@@ -226,10 +226,6 @@
   </si>
   <si>
     <t>DVD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>98´</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -630,10 +626,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>66´05"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Dziga Vertov</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -649,18 +641,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>78´16"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Robert J. Flaherty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Charles Gelb / Robert J. Flaherty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Timothy Brock</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -845,9 +829,6 @@
     <t>VHS</t>
   </si>
   <si>
-    <t>Registros fílmicos, ficción</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Usos reservados para consulta </t>
     </r>
@@ -915,10 +896,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>50´</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Basil Emmott</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -947,18 +924,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Nogent, Marne</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>35 mm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>17´</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Pelicula muda</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -970,9 +939,6 @@
   </si>
   <si>
     <t>Película documental</t>
-  </si>
-  <si>
-    <t>Grabación de campo, cartografía</t>
   </si>
   <si>
     <t xml:space="preserve">(http://www.divisared.es/index.aspx)   Información General:  divisa@divisared.es  Prensa y Comunicación: prensa@divisared.es    DIVISA HOME VIDEO® 
@@ -1066,10 +1032,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>12"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Joris Ivens, Mannus H. K. Franken</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1095,12 +1057,6 @@
   </si>
   <si>
     <t>Esteban Terán (Área de contexto)</t>
-  </si>
-  <si>
-    <t>Última modificación: 11/03/2013</t>
-  </si>
-  <si>
-    <t>Úrsula Mares</t>
   </si>
   <si>
     <t>La primera película de Carné, filmada a los 20 años y que trata de de los placeres simples de la gente sencilla en una tarde de domingo, cerca de París, a las orillas del río Marne. Carné filmó su película con la ayuda de Michel Sanvoisin, un relojero de cierto renombre en el mundo del cine aficionado: Sanvoisin le dio la cámara y película, y también participó en la filmación. http://scalisto.blogspot.mx/2011/01/marcel-carne-nogent-eldorado-du.html                                                                                    Otra sinopsis en francés: http://www.marcel-carne.com/les-films-de-marcel-carne/1929-nogent-eldorado-du-dimanche/fiche-technique-synopsis-revue-de-presse/</t>
@@ -1145,9 +1101,6 @@
     </r>
   </si>
   <si>
-    <t>Antes habían 2 DVD´s ahora aparece 1.</t>
-  </si>
-  <si>
     <t>1 dvd / 1 vhs</t>
   </si>
   <si>
@@ -1186,6 +1139,93 @@
   </si>
   <si>
     <t xml:space="preserve">Hay dos dvds, el tono en el que se ven es virado a azul. http://metamentaldoc.com/ft_grierson.pdf </t>
+  </si>
+  <si>
+    <t>50'</t>
+  </si>
+  <si>
+    <t>98'</t>
+  </si>
+  <si>
+    <t>78'16''</t>
+  </si>
+  <si>
+    <t>Charles Gelb, Robert J. Flaherty</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ficción, registros videográficos, fotografía, </t>
+  </si>
+  <si>
+    <t>Rusia: San Petesburgo</t>
+  </si>
+  <si>
+    <t>Chelovek kinoapparatom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 dvd, 1 vhs </t>
+  </si>
+  <si>
+    <t>Esteban Terán (Área de contexto), Penélope Ubaldo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros fílmicos, ficción, registros fílmicos, </t>
+  </si>
+  <si>
+    <t>Nogent, el dorado du diamanche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grabación de campo, cartografía, intertítulos, </t>
+  </si>
+  <si>
+    <t>Flaherty y otros títulos,  ficha técnica.</t>
+  </si>
+  <si>
+    <t>Nanook of the north</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01/07/2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29/06/2015</t>
+  </si>
+  <si>
+    <t>No se encuentra en el acervo físico</t>
+  </si>
+  <si>
+    <t>En el mismo DVD, se encuentran tres títulos "A Valparaíso" 26'38'', Nogent 14'57'' y Van Gogh 17'55''</t>
+  </si>
+  <si>
+    <t>Michel Sanvoisin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hortensia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Francés </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grabación de campo, intertítulos, música de época </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nogent, Marne, Casino de Tremblay, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros fílmicos, ficción, </t>
+  </si>
+  <si>
+    <t>15'</t>
+  </si>
+  <si>
+    <t>Úrsula Mares, Penélope Ubaldo</t>
+  </si>
+  <si>
+    <t>11'</t>
+  </si>
+  <si>
+    <t>65'45''</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1325,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1319,6 +1359,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1396,7 +1442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1476,9 +1522,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1513,6 +1556,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1547,6 +1593,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1885,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="67" zoomScaleNormal="67" zoomScalePageLayoutView="67" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" zoomScalePageLayoutView="67" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1921,7 +1970,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -1952,7 +2001,7 @@
     <row r="2" spans="1:26" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="62"/>
@@ -1962,7 +2011,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="15"/>
       <c r="J2" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" s="58"/>
       <c r="L2" s="58"/>
@@ -1973,11 +2022,11 @@
       <c r="Q2" s="58"/>
       <c r="R2" s="57"/>
       <c r="S2" s="56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T2" s="57"/>
       <c r="U2" s="56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V2" s="57"/>
       <c r="W2" s="13"/>
@@ -1987,122 +2036,122 @@
     </row>
     <row r="3" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="D3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="30" t="s">
-        <v>38</v>
-      </c>
       <c r="E3" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="30" t="s">
+      <c r="H3" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="I3" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="J3" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="30" t="s">
+      <c r="O3" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="P3" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="Q3" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="R3" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="30" t="s">
-        <v>54</v>
-      </c>
       <c r="S3" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="T3" s="30" t="s">
-        <v>57</v>
-      </c>
       <c r="U3" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="V3" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="30" t="s">
+      <c r="W3" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="W3" s="30" t="s">
+      <c r="X3" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="X3" s="30" t="s">
+      <c r="Y3" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="Y3" s="30" t="s">
+      <c r="Z3" s="30" t="s">
         <v>64</v>
-      </c>
-      <c r="Z3" s="30" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="72.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>100</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H4" s="17">
         <v>1929</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>109</v>
+        <v>222</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
@@ -2115,38 +2164,38 @@
     </row>
     <row r="5" spans="1:26" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H5" s="17">
         <v>1929</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>142</v>
+        <v>194</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="17" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
@@ -2159,29 +2208,29 @@
     </row>
     <row r="6" spans="1:26" ht="66.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" s="17">
         <v>1924</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>32</v>
+        <v>195</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="17" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="17"/>
@@ -2203,142 +2252,144 @@
     </row>
     <row r="7" spans="1:26" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H7" s="17">
         <v>1922</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>114</v>
+        <v>196</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q7" s="4"/>
       <c r="R7" s="17" t="s">
-        <v>116</v>
+        <v>197</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="4"/>
       <c r="Z7" s="17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="17">
         <v>1929</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="J8" s="4"/>
+        <v>219</v>
+      </c>
+      <c r="J8" s="17"/>
       <c r="K8" s="17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="V8" s="4"/>
+        <v>143</v>
+      </c>
+      <c r="V8" s="17" t="s">
+        <v>214</v>
+      </c>
       <c r="W8" s="4"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="17" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="60.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="17" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="H9" s="17">
         <v>1929</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>182</v>
+        <v>221</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="17" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="17" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="17" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="17" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -2387,8 +2438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="56" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A7" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="56" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2405,45 +2456,45 @@
   <sheetData>
     <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
       <c r="D1" s="59"/>
       <c r="E1" s="59"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="60" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="62"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="50"/>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="D3" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>77</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>78</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>15</v>
@@ -2460,28 +2511,28 @@
     </row>
     <row r="4" spans="1:9" ht="298.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>187</v>
+        <v>98</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>177</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I4" s="17">
         <v>1999</v>
@@ -2489,76 +2540,76 @@
     </row>
     <row r="5" spans="1:9" ht="334.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="52"/>
+        <v>97</v>
+      </c>
+      <c r="D5" s="51"/>
       <c r="E5" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="53"/>
+      <c r="H5" s="52"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="273" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>188</v>
+        <v>101</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>178</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="H6" s="53"/>
+        <v>118</v>
+      </c>
+      <c r="H6" s="52"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="273.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>0</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I7" s="17">
         <v>1999</v>
@@ -2566,49 +2617,49 @@
     </row>
     <row r="8" spans="1:9" ht="262.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
+        <v>103</v>
+      </c>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
       <c r="G8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="53"/>
+      <c r="H8" s="52"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="195.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D9" s="53"/>
+        <v>158</v>
+      </c>
+      <c r="D9" s="52"/>
       <c r="E9" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
+        <v>173</v>
+      </c>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="54"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2634,8 +2685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="66" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A9" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="66" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2656,7 +2707,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -2680,7 +2731,7 @@
       <c r="E2" s="61"/>
       <c r="F2" s="62"/>
       <c r="G2" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
@@ -2690,10 +2741,10 @@
     </row>
     <row r="3" spans="1:13" ht="56.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>19</v>
@@ -2720,62 +2771,72 @@
         <v>27</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="292.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="17" t="s">
+        <v>200</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="I4" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="J4" s="1"/>
+        <v>218</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>199</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="17" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>204</v>
+      </c>
       <c r="J5" s="17" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -2783,28 +2844,28 @@
     </row>
     <row r="6" spans="1:13" ht="170.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="17" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="17" t="s">
         <v>29</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -2812,96 +2873,100 @@
     </row>
     <row r="7" spans="1:13" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>103</v>
+        <v>208</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="1"/>
       <c r="J7" s="17" t="s">
-        <v>157</v>
+        <v>206</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="M7" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="146.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>181</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>213</v>
+      </c>
       <c r="E8" s="17" t="s">
-        <v>150</v>
+        <v>217</v>
       </c>
       <c r="F8" s="17">
         <v>1929</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="17" t="s">
-        <v>145</v>
+        <v>216</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="17" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="138.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="17" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F9" s="17">
         <v>1929</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="17" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="17" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="M9" s="1"/>
     </row>
@@ -2931,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="66" zoomScalePageLayoutView="66" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="H7" zoomScale="75" zoomScaleNormal="66" zoomScalePageLayoutView="66" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2957,7 +3022,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="56.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -2965,7 +3030,7 @@
       <c r="E1" s="64"/>
       <c r="F1" s="26"/>
       <c r="G1" s="18"/>
-      <c r="H1" s="45"/>
+      <c r="H1" s="44"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
@@ -2980,12 +3045,12 @@
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
       <c r="E2" s="60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="61"/>
       <c r="G2" s="61"/>
       <c r="H2" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I2" s="61"/>
       <c r="J2" s="61"/>
@@ -2997,28 +3062,28 @@
     </row>
     <row r="3" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="30" t="s">
-        <v>84</v>
-      </c>
       <c r="E3" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="G3" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="30" t="s">
-        <v>88</v>
-      </c>
       <c r="H3" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>5</v>
@@ -3027,34 +3092,34 @@
         <v>6</v>
       </c>
       <c r="K3" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="M3" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="M3" s="30" t="s">
+      <c r="N3" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="O3" s="30" t="s">
         <v>94</v>
-      </c>
-      <c r="O3" s="30" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -3062,17 +3127,17 @@
         <v>1</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="J4" s="17" t="s">
         <v>7</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="17" t="s">
@@ -3081,22 +3146,22 @@
     </row>
     <row r="5" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="17" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="17" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>8</v>
@@ -3105,28 +3170,28 @@
         <v>9</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="66.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="17" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="17" t="s">
@@ -3138,55 +3203,55 @@
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="17" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="O7" s="17" t="s">
         <v>4</v>
@@ -3194,22 +3259,24 @@
     </row>
     <row r="8" spans="1:15" ht="60.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="17" t="s">
+        <v>215</v>
+      </c>
       <c r="H8" s="17" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>11</v>
@@ -3218,48 +3285,48 @@
         <v>12</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="17" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="17" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3285,8 +3352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3299,7 +3366,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -3315,27 +3382,27 @@
     </row>
     <row r="3" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>67</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3343,10 +3410,10 @@
     </row>
     <row r="5" spans="1:5" ht="60.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -3354,10 +3421,10 @@
     </row>
     <row r="6" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -3365,10 +3432,10 @@
     </row>
     <row r="7" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -3376,10 +3443,10 @@
     </row>
     <row r="8" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -3387,10 +3454,10 @@
     </row>
     <row r="9" spans="1:5" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -3417,8 +3484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3430,7 +3497,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="67"/>
@@ -3442,77 +3509,79 @@
     </row>
     <row r="3" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="75.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="54" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="78.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="75.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>204</v>
+        <v>101</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3537,7 +3606,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3551,7 +3620,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -3569,130 +3638,132 @@
     </row>
     <row r="3" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>72</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" s="44" t="s">
-        <v>191</v>
+        <v>203</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="55">
+        <v>40722</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>191</v>
+        <v>203</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="17"/>
+        <v>101</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>211</v>
+      </c>
       <c r="D6" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>191</v>
+        <v>180</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="F6" s="55">
+        <v>39882</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="48.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="F7" s="44" t="s">
-        <v>191</v>
+        <v>203</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="51.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="F8" s="43">
-        <v>39711</v>
+        <v>220</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" s="43">
-        <v>39711</v>
+        <v>220</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix para inserciones automaticas desde csv
</commit_message>
<xml_diff>
--- a/content/excel/Fichas década4 (1920).xlsx
+++ b/content/excel/Fichas década4 (1920).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19320" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19320" windowHeight="15480" tabRatio="500" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ÁREA DE IDENTIFICACIÓN" sheetId="1" r:id="rId1"/>
@@ -981,10 +981,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Se encuentra ubicado en la caja que dice "Hacer copia  Une histoire de vent"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Reproductor DVD y Monitor </t>
   </si>
   <si>
@@ -1226,6 +1222,9 @@
   </si>
   <si>
     <t>65'45''</t>
+  </si>
+  <si>
+    <t>Se encuentra ubicado en la caja que dice "Hacer copia  Une histoire de vent"</t>
   </si>
 </sst>
 </file>
@@ -1559,6 +1558,9 @@
     <xf numFmtId="14" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1593,9 +1595,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1934,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" zoomScalePageLayoutView="67" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScale="67" zoomScaleNormal="67" zoomScalePageLayoutView="67" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1969,13 +1968,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
@@ -2000,35 +1999,35 @@
     </row>
     <row r="2" spans="1:26" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="15"/>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="56" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="56" t="s">
+      <c r="T2" s="58"/>
+      <c r="U2" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="V2" s="57"/>
+      <c r="V2" s="58"/>
       <c r="W2" s="13"/>
       <c r="X2" s="13"/>
       <c r="Y2" s="12"/>
@@ -2116,10 +2115,10 @@
     </row>
     <row r="4" spans="1:26" ht="72.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>99</v>
@@ -2134,7 +2133,7 @@
         <v>1929</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="17" t="s">
@@ -2180,7 +2179,7 @@
         <v>1929</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="17" t="s">
@@ -2211,7 +2210,7 @@
         <v>130</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>32</v>
@@ -2226,11 +2225,11 @@
         <v>1924</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="17"/>
@@ -2270,7 +2269,7 @@
         <v>1922</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="17" t="s">
@@ -2287,7 +2286,7 @@
       </c>
       <c r="Q7" s="4"/>
       <c r="R7" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
@@ -2322,7 +2321,7 @@
         <v>1929</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17" t="s">
@@ -2343,7 +2342,7 @@
         <v>143</v>
       </c>
       <c r="V8" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W8" s="4"/>
       <c r="X8" s="2"/>
@@ -2354,10 +2353,10 @@
     </row>
     <row r="9" spans="1:26" ht="60.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>156</v>
@@ -2366,21 +2365,21 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H9" s="17">
         <v>1929</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -2455,13 +2454,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="A1" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="46"/>
       <c r="G1" s="46"/>
       <c r="H1" s="46"/>
@@ -2470,11 +2469,11 @@
     <row r="2" spans="1:9" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="47"/>
       <c r="B2" s="48"/>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="47"/>
       <c r="G2" s="49"/>
       <c r="H2" s="50"/>
@@ -2511,22 +2510,22 @@
     </row>
     <row r="4" spans="1:9" ht="298.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>98</v>
       </c>
       <c r="C4" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>178</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>179</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>118</v>
@@ -2569,16 +2568,16 @@
         <v>101</v>
       </c>
       <c r="C6" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="E6" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>178</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>179</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>118</v>
@@ -2634,17 +2633,17 @@
     </row>
     <row r="9" spans="1:9" ht="195.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>158</v>
       </c>
       <c r="D9" s="52"/>
       <c r="E9" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
@@ -2685,8 +2684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="66" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="66" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2706,13 +2705,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="63"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="64"/>
       <c r="F1" s="33"/>
       <c r="G1" s="34"/>
       <c r="H1" s="34"/>
@@ -2725,19 +2724,19 @@
       <c r="A2" s="31"/>
       <c r="B2" s="14"/>
       <c r="C2" s="32"/>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="60" t="s">
+      <c r="E2" s="62"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="63"/>
     </row>
     <row r="3" spans="1:13" ht="56.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
@@ -2777,35 +2776,35 @@
         <v>79</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="292.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>98</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="17" t="s">
         <v>119</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="J4" s="17" t="s">
         <v>198</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>199</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="17" t="s">
@@ -2821,7 +2820,7 @@
         <v>100</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2830,10 +2829,10 @@
         <v>135</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>139</v>
@@ -2850,10 +2849,10 @@
         <v>101</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2876,16 +2875,16 @@
         <v>134</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>146</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>147</v>
@@ -2896,14 +2895,14 @@
       <c r="H7" s="17"/>
       <c r="I7" s="1"/>
       <c r="J7" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="146.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2911,16 +2910,16 @@
         <v>132</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F8" s="17">
         <v>1929</v>
@@ -2931,7 +2930,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="17" t="s">
@@ -2941,17 +2940,17 @@
     </row>
     <row r="9" spans="1:13" ht="138.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>155</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F9" s="17">
         <v>1929</v>
@@ -2962,7 +2961,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="17" t="s">
@@ -3021,13 +3020,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="56.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
       <c r="F1" s="26"/>
       <c r="G1" s="18"/>
       <c r="H1" s="44"/>
@@ -3044,19 +3043,19 @@
       <c r="B2" s="11"/>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="60" t="s">
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
       <c r="N2" s="7"/>
       <c r="O2" s="8"/>
     </row>
@@ -3109,7 +3108,7 @@
     </row>
     <row r="4" spans="1:15" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>98</v>
@@ -3127,7 +3126,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J4" s="17" t="s">
         <v>7</v>
@@ -3156,12 +3155,12 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>8</v>
@@ -3170,13 +3169,13 @@
         <v>9</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="66.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3191,7 +3190,7 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="17" t="s">
@@ -3203,13 +3202,13 @@
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3236,7 +3235,7 @@
         <v>3</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>10</v>
@@ -3273,7 +3272,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>154</v>
@@ -3291,15 +3290,15 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>121</v>
@@ -3314,10 +3313,10 @@
         <v>154</v>
       </c>
       <c r="I9" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="J9" s="17" t="s">
         <v>183</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>184</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>123</v>
@@ -3326,7 +3325,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3352,8 +3351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3365,13 +3364,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
@@ -3399,7 +3398,7 @@
     </row>
     <row r="4" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>98</v>
@@ -3454,10 +3453,10 @@
     </row>
     <row r="9" spans="1:5" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -3485,7 +3484,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3496,11 +3495,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="67"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
@@ -3520,13 +3519,13 @@
     </row>
     <row r="4" spans="1:3" ht="75.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>98</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="78.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3537,7 +3536,7 @@
         <v>100</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="75.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3547,8 +3546,8 @@
       <c r="B6" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="68" t="s">
-        <v>191</v>
+      <c r="C6" s="56" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -3559,7 +3558,7 @@
         <v>102</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -3570,18 +3569,18 @@
         <v>103</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -3606,7 +3605,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3619,14 +3618,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="67"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="68"/>
     </row>
     <row r="2" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
@@ -3658,17 +3657,17 @@
     </row>
     <row r="4" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>98</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="55">
         <v>40722</v>
@@ -3683,13 +3682,13 @@
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -3699,14 +3698,14 @@
       <c r="B6" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="68" t="s">
-        <v>211</v>
+      <c r="C6" s="56" t="s">
+        <v>210</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F6" s="55">
         <v>39882</v>
@@ -3721,13 +3720,13 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="51.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3739,31 +3738,31 @@
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>